<commit_message>
Correction du bug 5 des test boite noir et d'autre correction de la revu de code
</commit_message>
<xml_diff>
--- a/TP1/revue_code/revue_code_SCEP.xlsx
+++ b/TP1/revue_code/revue_code_SCEP.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20378"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D77606BF-DB03-470C-B8DE-60B5224DDF35}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B5CEADE-FC07-4F70-AC1F-24E77EA3CE2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17565" yWindow="4650" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="64">
   <si>
     <t>FICHE DE RÉVISION DE CODE</t>
   </si>
@@ -206,6 +206,12 @@
   </si>
   <si>
     <t>Mettre une ligne vide</t>
+  </si>
+  <si>
+    <t>Amar</t>
+  </si>
+  <si>
+    <t>Corrigé</t>
   </si>
 </sst>
 </file>
@@ -563,8 +569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -736,7 +742,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>4</v>
       </c>
@@ -752,8 +758,14 @@
       <c r="E17" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>62</v>
+      </c>
+      <c r="G17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>5</v>
       </c>
@@ -769,8 +781,14 @@
       <c r="E18" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" t="s">
+        <v>62</v>
+      </c>
+      <c r="G18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>6</v>
       </c>
@@ -787,7 +805,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>7</v>
       </c>
@@ -803,8 +821,14 @@
       <c r="E20" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
+        <v>62</v>
+      </c>
+      <c r="G20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>8</v>
       </c>
@@ -821,7 +845,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>9</v>
       </c>
@@ -837,8 +861,14 @@
       <c r="E22" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" t="s">
+        <v>62</v>
+      </c>
+      <c r="G22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>10</v>
       </c>
@@ -855,7 +885,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>11</v>
       </c>
@@ -872,7 +902,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>12</v>
       </c>
@@ -888,8 +918,14 @@
       <c r="E25" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25" t="s">
+        <v>62</v>
+      </c>
+      <c r="G25" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>13</v>
       </c>
@@ -906,7 +942,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>14</v>
       </c>
@@ -923,7 +959,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>15</v>
       </c>
@@ -940,7 +976,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>33</v>
       </c>
@@ -954,7 +990,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>35</v>
       </c>
@@ -968,7 +1004,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>16</v>
       </c>
@@ -985,7 +1021,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Travail correction (En cours)
</commit_message>
<xml_diff>
--- a/TP1/revue_code/revue_code_SCEP.xlsx
+++ b/TP1/revue_code/revue_code_SCEP.xlsx
@@ -1,26 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20378"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D77606BF-DB03-470C-B8DE-60B5224DDF35}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2CA3907-0885-4173-8C3D-B687D55295D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="63">
   <si>
     <t>FICHE DE RÉVISION DE CODE</t>
   </si>
@@ -206,6 +215,9 @@
   </si>
   <si>
     <t>Mettre une ligne vide</t>
+  </si>
+  <si>
+    <t>Mohamad</t>
   </si>
 </sst>
 </file>
@@ -563,20 +575,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="95" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="12.85546875" customWidth="1"/>
-    <col min="4" max="4" width="96.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.86328125" customWidth="1"/>
+    <col min="4" max="4" width="96.265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -587,7 +599,7 @@
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C3" t="s">
         <v>1</v>
       </c>
@@ -601,7 +613,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C4" t="s">
         <v>5</v>
       </c>
@@ -612,7 +624,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C5" t="s">
         <v>8</v>
       </c>
@@ -623,7 +635,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="D6" t="s">
         <v>49</v>
       </c>
@@ -631,22 +643,22 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="D7" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="D8" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="D9" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C10" t="s">
         <v>12</v>
       </c>
@@ -654,7 +666,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C12" s="1" t="s">
         <v>13</v>
       </c>
@@ -662,7 +674,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="2" t="s">
         <v>15</v>
       </c>
@@ -685,7 +697,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>1</v>
       </c>
@@ -702,8 +714,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15">
+        <f>A14+1</f>
         <v>2</v>
       </c>
       <c r="B15">
@@ -719,8 +732,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16">
+        <f t="shared" ref="A16:A55" si="0">A15+1</f>
         <v>3</v>
       </c>
       <c r="B16">
@@ -736,8 +750,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B17">
@@ -752,9 +767,13 @@
       <c r="E17" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B18">
@@ -769,9 +788,13 @@
       <c r="E18" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B19">
@@ -787,8 +810,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B20">
@@ -803,9 +827,13 @@
       <c r="E20" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B21">
@@ -821,8 +849,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22">
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B22">
@@ -837,9 +866,13 @@
       <c r="E22" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B23">
@@ -855,8 +888,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24">
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B24">
@@ -872,8 +906,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B25">
@@ -888,9 +923,13 @@
       <c r="E25" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26">
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B26">
@@ -906,8 +945,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27">
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B27">
@@ -923,8 +963,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28">
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B28">
@@ -940,7 +981,11 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A29">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
       <c r="B29">
         <v>33</v>
       </c>
@@ -954,7 +999,11 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A30">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
       <c r="B30">
         <v>35</v>
       </c>
@@ -967,10 +1016,14 @@
       <c r="E30" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31">
-        <v>16</v>
+        <f t="shared" si="0"/>
+        <v>18</v>
       </c>
       <c r="B31">
         <v>41</v>
@@ -985,9 +1038,10 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32">
-        <v>17</v>
+        <f t="shared" si="0"/>
+        <v>19</v>
       </c>
       <c r="B32">
         <v>41</v>
@@ -1002,9 +1056,10 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33">
-        <v>18</v>
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
       <c r="B33">
         <v>43</v>
@@ -1019,9 +1074,10 @@
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34">
-        <v>19</v>
+        <f t="shared" si="0"/>
+        <v>21</v>
       </c>
       <c r="B34">
         <v>45</v>
@@ -1035,10 +1091,14 @@
       <c r="E34" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F34" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35">
-        <v>20</v>
+        <f t="shared" si="0"/>
+        <v>22</v>
       </c>
       <c r="B35">
         <v>46</v>
@@ -1052,10 +1112,14 @@
       <c r="E35" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F35" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36">
-        <v>21</v>
+        <f t="shared" si="0"/>
+        <v>23</v>
       </c>
       <c r="B36">
         <v>47</v>
@@ -1069,10 +1133,14 @@
       <c r="E36" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F36" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37">
-        <v>22</v>
+        <f t="shared" si="0"/>
+        <v>24</v>
       </c>
       <c r="B37">
         <v>47</v>
@@ -1087,9 +1155,10 @@
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38">
-        <v>23</v>
+        <f t="shared" si="0"/>
+        <v>25</v>
       </c>
       <c r="B38">
         <v>48</v>
@@ -1104,9 +1173,10 @@
         <v>24</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39">
-        <v>24</v>
+        <f t="shared" si="0"/>
+        <v>26</v>
       </c>
       <c r="B39">
         <v>48</v>
@@ -1121,9 +1191,10 @@
         <v>27</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40">
-        <v>25</v>
+        <f t="shared" si="0"/>
+        <v>27</v>
       </c>
       <c r="B40">
         <v>51</v>
@@ -1138,9 +1209,10 @@
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41">
-        <v>26</v>
+        <f t="shared" si="0"/>
+        <v>28</v>
       </c>
       <c r="B41">
         <v>51</v>
@@ -1155,9 +1227,10 @@
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42">
-        <v>27</v>
+        <f t="shared" si="0"/>
+        <v>29</v>
       </c>
       <c r="B42">
         <v>58</v>
@@ -1172,9 +1245,10 @@
         <v>24</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43">
-        <v>28</v>
+        <f t="shared" si="0"/>
+        <v>30</v>
       </c>
       <c r="B43">
         <v>58</v>
@@ -1189,9 +1263,10 @@
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44">
-        <v>29</v>
+        <f t="shared" si="0"/>
+        <v>31</v>
       </c>
       <c r="B44">
         <v>58</v>
@@ -1206,9 +1281,10 @@
         <v>27</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45">
-        <v>30</v>
+        <f t="shared" si="0"/>
+        <v>32</v>
       </c>
       <c r="B45">
         <v>61</v>
@@ -1223,9 +1299,10 @@
         <v>27</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46">
-        <v>31</v>
+        <f t="shared" si="0"/>
+        <v>33</v>
       </c>
       <c r="B46">
         <v>61</v>
@@ -1240,9 +1317,10 @@
         <v>27</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47">
-        <v>32</v>
+        <f t="shared" si="0"/>
+        <v>34</v>
       </c>
       <c r="B47">
         <v>61</v>
@@ -1257,9 +1335,10 @@
         <v>27</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48">
-        <v>33</v>
+        <f t="shared" si="0"/>
+        <v>35</v>
       </c>
       <c r="B48">
         <v>62</v>
@@ -1274,9 +1353,10 @@
         <v>24</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A49">
-        <v>34</v>
+        <f t="shared" si="0"/>
+        <v>36</v>
       </c>
       <c r="B49">
         <v>62</v>
@@ -1291,9 +1371,10 @@
         <v>27</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A50">
-        <v>35</v>
+        <f t="shared" si="0"/>
+        <v>37</v>
       </c>
       <c r="B50">
         <v>90</v>
@@ -1308,9 +1389,10 @@
         <v>27</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A51">
-        <v>36</v>
+        <f t="shared" si="0"/>
+        <v>38</v>
       </c>
       <c r="B51">
         <v>104</v>
@@ -1325,9 +1407,10 @@
         <v>24</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A52">
-        <v>37</v>
+        <f t="shared" si="0"/>
+        <v>39</v>
       </c>
       <c r="B52">
         <v>109</v>
@@ -1342,9 +1425,10 @@
         <v>27</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A53">
-        <v>38</v>
+        <f t="shared" si="0"/>
+        <v>40</v>
       </c>
       <c r="B53">
         <v>109</v>
@@ -1359,9 +1443,10 @@
         <v>24</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A54">
-        <v>39</v>
+        <f t="shared" si="0"/>
+        <v>41</v>
       </c>
       <c r="B54">
         <v>111</v>
@@ -1376,9 +1461,10 @@
         <v>27</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A55">
-        <v>40</v>
+        <f t="shared" si="0"/>
+        <v>42</v>
       </c>
       <c r="B55">
         <v>111</v>

</xml_diff>

<commit_message>
correction des erreurs de l'id 24 a 42
</commit_message>
<xml_diff>
--- a/TP1/revue_code/revue_code_SCEP.xlsx
+++ b/TP1/revue_code/revue_code_SCEP.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20378"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E1C7499-45EB-4EE3-A689-1E88D92D9CA6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC9B3E08-6E40-41F6-A630-A359E950EBCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="24495" windowHeight="15795" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5115" yWindow="3750" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="64">
   <si>
     <t>FICHE DE RÉVISION DE CODE</t>
   </si>
@@ -218,6 +218,9 @@
   </si>
   <si>
     <t>Mohamad</t>
+  </si>
+  <si>
+    <t>Amar</t>
   </si>
 </sst>
 </file>
@@ -575,8 +578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="95" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="E19" zoomScale="95" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1157,6 +1160,9 @@
       <c r="E37" t="s">
         <v>27</v>
       </c>
+      <c r="F37" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
@@ -1193,6 +1199,9 @@
       <c r="E39" t="s">
         <v>27</v>
       </c>
+      <c r="F39" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
@@ -1229,6 +1238,9 @@
       <c r="E41" t="s">
         <v>27</v>
       </c>
+      <c r="F41" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
@@ -1265,6 +1277,9 @@
       <c r="E43" t="s">
         <v>27</v>
       </c>
+      <c r="F43" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
@@ -1283,6 +1298,9 @@
       <c r="E44" t="s">
         <v>27</v>
       </c>
+      <c r="F44" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
@@ -1301,6 +1319,9 @@
       <c r="E45" t="s">
         <v>27</v>
       </c>
+      <c r="F45" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
@@ -1319,6 +1340,9 @@
       <c r="E46" t="s">
         <v>27</v>
       </c>
+      <c r="F46" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
@@ -1337,6 +1361,9 @@
       <c r="E47" t="s">
         <v>27</v>
       </c>
+      <c r="F47" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
@@ -1356,7 +1383,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -1373,8 +1400,11 @@
       <c r="E49" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F49" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -1391,8 +1421,11 @@
       <c r="E50" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F50" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -1410,7 +1443,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -1427,8 +1460,11 @@
       <c r="E52" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F52" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -1446,7 +1482,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -1463,8 +1499,11 @@
       <c r="E54" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F54" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -1480,6 +1519,9 @@
       </c>
       <c r="E55" t="s">
         <v>27</v>
+      </c>
+      <c r="F55" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>